<commit_message>
fsm and procedure manager
</commit_message>
<xml_diff>
--- a/Factorio/resource/datatables/datatable.xlsx
+++ b/Factorio/resource/datatables/datatable.xlsx
@@ -96,7 +96,7 @@
     <t>铁板</t>
   </si>
   <si>
-    <t>Gear</t>
+    <t>GEAR</t>
   </si>
   <si>
     <t>gear</t>
@@ -1147,7 +1147,7 @@
   <dimension ref="A1:WQV15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
basic building tool / selection / main tile map
</commit_message>
<xml_diff>
--- a/Factorio/resource/datatables/datatable.xlsx
+++ b/Factorio/resource/datatables/datatable.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22410" windowHeight="13560" activeTab="2"/>
+    <workbookView windowWidth="30240" windowHeight="8535" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="item_type" sheetId="2" r:id="rId1"/>
     <sheet name="items" sheetId="1" r:id="rId2"/>
-    <sheet name="construct" sheetId="3" r:id="rId3"/>
+    <sheet name="tilemap" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="83">
   <si>
     <t>id</t>
   </si>
@@ -184,13 +184,25 @@
     <t>size</t>
   </si>
   <si>
-    <t>tilemap_source_id</t>
+    <t>source_id</t>
   </si>
   <si>
-    <t>tilemap_layer_name</t>
+    <t>layer_name</t>
   </si>
   <si>
-    <t>atlas_coordinates</t>
+    <t>atlas_coords</t>
+  </si>
+  <si>
+    <t>size_in_atlas</t>
+  </si>
+  <si>
+    <t>texture_origin</t>
+  </si>
+  <si>
+    <t>collision_poly</t>
+  </si>
+  <si>
+    <t>selection_poly</t>
   </si>
   <si>
     <t>尺寸</t>
@@ -202,10 +214,25 @@
     <t>坐标</t>
   </si>
   <si>
+    <t>图形尺寸</t>
+  </si>
+  <si>
+    <t>贴图中心</t>
+  </si>
+  <si>
+    <t>碰撞区域</t>
+  </si>
+  <si>
+    <t>选择区域</t>
+  </si>
+  <si>
     <t>Vector2i</t>
   </si>
   <si>
-    <t>1,2</t>
+    <t>list[int]</t>
+  </si>
+  <si>
+    <t>1,1</t>
   </si>
   <si>
     <t>Entity</t>
@@ -214,16 +241,43 @@
     <t>9,0</t>
   </si>
   <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>0,16</t>
+  </si>
+  <si>
+    <t>4,36,4,4</t>
+  </si>
+  <si>
+    <t>0,32,0,0</t>
+  </si>
+  <si>
     <t>2,2</t>
   </si>
   <si>
     <t>2,3</t>
   </si>
   <si>
+    <t>-16,-16</t>
+  </si>
+  <si>
+    <t>4,4,4,4</t>
+  </si>
+  <si>
+    <t>0,0,0,0</t>
+  </si>
+  <si>
     <t>3,3</t>
   </si>
   <si>
     <t>0,5</t>
+  </si>
+  <si>
+    <t>-32,-32</t>
+  </si>
+  <si>
+    <t>0,3</t>
   </si>
 </sst>
 </file>
@@ -888,6 +942,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1280,7 +1337,7 @@
   <dimension ref="A1:WQV15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -17518,22 +17575,24 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6"/>
   <cols>
     <col min="1" max="1" width="23.75" customWidth="1"/>
     <col min="2" max="2" width="13.125" customWidth="1"/>
     <col min="3" max="3" width="24.125" customWidth="1"/>
     <col min="4" max="4" width="20.375" customWidth="1"/>
-    <col min="5" max="5" width="26.75" customWidth="1"/>
+    <col min="5" max="5" width="25.625" customWidth="1"/>
+    <col min="6" max="8" width="32" customWidth="1"/>
+    <col min="9" max="9" width="20.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:5">
+    <row r="1" s="1" customFormat="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -17549,30 +17608,54 @@
       <c r="E1" s="1" t="s">
         <v>53</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="2" s="1" customFormat="1" spans="1:5">
+    <row r="2" s="1" customFormat="1" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" spans="1:5">
+    <row r="3" s="1" customFormat="1" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
@@ -17581,58 +17664,135 @@
         <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>57</v>
+        <v>65</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="E4" t="s">
-        <v>60</v>
+        <v>69</v>
+      </c>
+      <c r="F4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I4" t="s">
+        <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
+        <v>75</v>
+      </c>
+      <c r="F5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H5" t="s">
+        <v>77</v>
+      </c>
+      <c r="I5" t="s">
+        <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="E6" t="s">
-        <v>64</v>
+        <v>80</v>
+      </c>
+      <c r="F6" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="H6" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H7" t="s">
+        <v>77</v>
+      </c>
+      <c r="I7" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
base inserter and chest inventory ui
</commit_message>
<xml_diff>
--- a/Factorio/resource/datatables/datatable.xlsx
+++ b/Factorio/resource/datatables/datatable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30240" windowHeight="8535" activeTab="2"/>
+    <workbookView windowWidth="30240" windowHeight="6180" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="item_type" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="85">
   <si>
     <t>id</t>
   </si>
@@ -278,6 +278,12 @@
   </si>
   <si>
     <t>0,3</t>
+  </si>
+  <si>
+    <t>6,2</t>
+  </si>
+  <si>
+    <t>0,0</t>
   </si>
 </sst>
 </file>
@@ -1337,7 +1343,7 @@
   <dimension ref="A1:WQV15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -17575,13 +17581,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7"/>
   <cols>
     <col min="1" max="1" width="23.75" customWidth="1"/>
     <col min="2" max="2" width="13.125" customWidth="1"/>
@@ -17795,6 +17801,35 @@
         <v>78</v>
       </c>
     </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" t="s">
+        <v>84</v>
+      </c>
+      <c r="H8" t="s">
+        <v>77</v>
+      </c>
+      <c r="I8" t="s">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
refactor inventory and base entity
</commit_message>
<xml_diff>
--- a/Factorio/resource/datatables/datatable.xlsx
+++ b/Factorio/resource/datatables/datatable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30240" windowHeight="6180" activeTab="2"/>
+    <workbookView windowWidth="30240" windowHeight="6180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="item_type" sheetId="2" r:id="rId1"/>
@@ -29,36 +29,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="94">
+  <si>
+    <t>name</t>
+  </si>
   <si>
     <t>id</t>
   </si>
   <si>
-    <t>name</t>
+    <t>名称</t>
   </si>
   <si>
     <t>ID</t>
   </si>
   <si>
-    <t>名称</t>
+    <t>string</t>
   </si>
   <si>
     <t>int</t>
   </si>
   <si>
-    <t>string</t>
+    <t>NATURAL_RESOURCES</t>
   </si>
   <si>
-    <t>natural_resources</t>
+    <t>LOGISTICS</t>
   </si>
   <si>
-    <t>logistics</t>
+    <t>PRODUCTIONS</t>
   </si>
   <si>
-    <t>productions</t>
-  </si>
-  <si>
-    <t>intermedia_products</t>
+    <t>INTERMEDIA_PRODUCTS</t>
   </si>
   <si>
     <t>__comment</t>
@@ -67,10 +67,31 @@
     <t>type</t>
   </si>
   <si>
+    <t>constructable</t>
+  </si>
+  <si>
+    <t>texture</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
     <t>注释</t>
   </si>
   <si>
     <t>资源类型</t>
+  </si>
+  <si>
+    <t>能否建造</t>
+  </si>
+  <si>
+    <t>贴图</t>
+  </si>
+  <si>
+    <t>图标</t>
+  </si>
+  <si>
+    <t>bool</t>
   </si>
   <si>
     <t>COAL</t>
@@ -236,9 +257,6 @@
   </si>
   <si>
     <t>list[int]</t>
-  </si>
-  <si>
-    <t>bool</t>
   </si>
   <si>
     <t>1,1</t>
@@ -1274,12 +1292,12 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="11.375" customWidth="1"/>
+    <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="26.375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1308,35 +1326,35 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
         <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
         <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
         <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
         <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1349,10 +1367,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:WQV15"/>
+  <dimension ref="A1:WQT15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1360,14 +1378,17 @@
     <col min="1" max="1" width="21.875" customWidth="1"/>
     <col min="2" max="3" width="31" customWidth="1"/>
     <col min="4" max="4" width="16.375" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="6" max="6" width="19.25" customWidth="1"/>
+    <col min="7" max="7" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>10</v>
@@ -1375,49 +1396,78 @@
       <c r="D1" t="s">
         <v>11</v>
       </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
+      <c r="E3" t="s">
+        <v>20</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
+      <c r="F3" t="s">
+        <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:16012">
+    <row r="4" spans="1:16010">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -17423,161 +17473,192 @@
       <c r="WQR4" s="2"/>
       <c r="WQS4" s="2"/>
       <c r="WQT4" s="2"/>
-      <c r="WQU4" s="2"/>
-      <c r="WQV4" s="2"/>
     </row>
-    <row r="5" s="2" customFormat="1" spans="1:4">
+    <row r="5" s="2" customFormat="1" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
       </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" s="2" customFormat="1" spans="1:4">
+    <row r="6" s="2" customFormat="1" spans="1:5">
       <c r="A6" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
       </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" s="3" customFormat="1" spans="1:4">
+    <row r="7" s="3" customFormat="1" spans="1:5">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D7" s="3">
         <v>4</v>
       </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" s="3" customFormat="1" spans="1:4">
+    <row r="8" s="3" customFormat="1" spans="1:5">
       <c r="A8" s="3" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="D8" s="3">
         <v>4</v>
       </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" s="4" customFormat="1" spans="1:4">
+    <row r="9" s="4" customFormat="1" spans="1:5">
       <c r="A9" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D9" s="4">
         <v>2</v>
       </c>
+      <c r="E9" s="4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" s="4" customFormat="1" spans="1:4">
+    <row r="10" s="4" customFormat="1" spans="1:5">
       <c r="A10" s="4" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="D10" s="4">
         <v>2</v>
       </c>
+      <c r="E10" s="4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="11" s="4" customFormat="1" spans="1:4">
+    <row r="11" s="4" customFormat="1" spans="1:5">
       <c r="A11" s="4" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="D11" s="4">
         <v>2</v>
       </c>
+      <c r="E11" s="4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="12" s="4" customFormat="1" spans="1:4">
+    <row r="12" s="4" customFormat="1" spans="1:5">
       <c r="A12" s="4" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D12" s="4">
         <v>2</v>
       </c>
+      <c r="E12" s="4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="13" s="5" customFormat="1" spans="1:4">
+    <row r="13" s="5" customFormat="1" spans="1:5">
       <c r="A13" s="5" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="D13" s="5">
         <v>3</v>
       </c>
+      <c r="E13" s="5">
+        <v>1</v>
+      </c>
     </row>
-    <row r="14" s="5" customFormat="1" spans="1:4">
+    <row r="14" s="5" customFormat="1" spans="1:5">
       <c r="A14" s="5" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D14" s="5">
         <v>3</v>
       </c>
+      <c r="E14" s="5">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" s="5" customFormat="1" spans="1:4">
+    <row r="15" s="5" customFormat="1" spans="1:5">
       <c r="A15" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D15" s="5">
         <v>3</v>
+      </c>
+      <c r="E15" s="5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -17592,7 +17673,7 @@
   <sheetPr/>
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -17610,127 +17691,127 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" spans="1:10">
       <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="E4" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="F4" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="G4" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="H4" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="I4" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -17738,31 +17819,31 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="E5" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="F5" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="H5" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="I5" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -17770,31 +17851,31 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="E6" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="F6" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="H6" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="I6" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -17802,31 +17883,31 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="E7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F7" t="s">
+        <v>83</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="F7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>79</v>
-      </c>
       <c r="H7" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="I7" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -17834,31 +17915,31 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="E8" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H8" t="s">
         <v>86</v>
       </c>
-      <c r="F8" t="s">
-        <v>70</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="I8" t="s">
         <v>87</v>
-      </c>
-      <c r="H8" t="s">
-        <v>80</v>
-      </c>
-      <c r="I8" t="s">
-        <v>81</v>
       </c>
       <c r="J8">
         <v>1</v>

</xml_diff>